<commit_message>
Final Project - working
Final project files, plot is working. Still need to make it prettier
</commit_message>
<xml_diff>
--- a/Final Project/Magnet Cove U-Pb Supplemental Data.xlsx
+++ b/Final Project/Magnet Cove U-Pb Supplemental Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brookepryor/Documents/School/GEOL 503 - Numerical Methods/Final Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brookepryor/Documents/GitHub/GEOL503FinalProjectSpring2025_BP/Final Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2442C022-59C7-EE45-93DA-40619FC862E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED0B602-7EE6-ED4A-B19B-FE35977A68C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{E8D1C77F-2FF3-7B43-9FD0-0EB2CB55D612}"/>
   </bookViews>
@@ -128,13 +128,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,7 +471,7 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -507,13 +506,13 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1">
-        <v>98.5</v>
+        <v>98.1</v>
       </c>
       <c r="C3" s="1">
-        <v>1.6</v>
+        <v>0.7</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
@@ -524,13 +523,13 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>98.1</v>
+        <v>98.5</v>
       </c>
       <c r="C4" s="1">
-        <v>0.7</v>
+        <v>1.6</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
@@ -541,13 +540,13 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1">
-        <v>102.8</v>
+        <v>101.4</v>
       </c>
       <c r="C5" s="1">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="D5" t="s">
         <v>3</v>
@@ -558,13 +557,13 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1">
-        <v>101.4</v>
+        <v>102.8</v>
       </c>
       <c r="C6" s="1">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="D6" t="s">
         <v>3</v>
@@ -574,13 +573,13 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="1">
         <v>96.4</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="1">
         <v>0.7</v>
       </c>
       <c r="D7" t="s">
@@ -591,13 +590,13 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="1">
         <v>97.2</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="1">
         <v>0.6</v>
       </c>
       <c r="D8" t="s">
@@ -608,13 +607,13 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="1">
         <v>97.3</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="1">
         <v>1.4</v>
       </c>
       <c r="D9" t="s">
@@ -642,60 +641,60 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
     </row>
     <row r="17" spans="10:14" x14ac:dyDescent="0.2">
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
     </row>
     <row r="18" spans="10:14" x14ac:dyDescent="0.2">
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
     </row>
     <row r="19" spans="10:14" x14ac:dyDescent="0.2">
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>